<commit_message>
Modified output to include a summary worksheet and a cell displaying total cost per cost centre
</commit_message>
<xml_diff>
--- a/model_inputs/cost_centres_and_sites/cost_centres_and_sites_reference.xlsx
+++ b/model_inputs/cost_centres_and_sites/cost_centres_and_sites_reference.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0FD7C4-23FB-46AA-B62E-311CCA664121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Centres" sheetId="1" r:id="rId1"/>
@@ -13,9 +12,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Centres'!$A$1:$D$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sites!$A$1:$F$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sites!$A$1:$F$138</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="359">
   <si>
     <t>BME_LMH</t>
   </si>
@@ -869,9 +868,6 @@
     <t>BROCK FAHRNI PAVILION (604) 806-9710</t>
   </si>
   <si>
-    <t>Biomed Eng - SPH</t>
-  </si>
-  <si>
     <t>EVDU</t>
   </si>
   <si>
@@ -1068,12 +1064,54 @@
   </si>
   <si>
     <t>imaging</t>
+  </si>
+  <si>
+    <t>SHHCC</t>
+  </si>
+  <si>
+    <t>SUNNY HILL HEALTH CENTRE FOR CHILDREN 604.453.8300</t>
+  </si>
+  <si>
+    <t>MHHO</t>
+  </si>
+  <si>
+    <t>DACSNE</t>
+  </si>
+  <si>
+    <t>EUPCC</t>
+  </si>
+  <si>
+    <t>EDMONDS URGENT PRIMARY CARE CENTER</t>
+  </si>
+  <si>
+    <t>DACSNE - DEPLOYABLE ALTERNATE CARE SITE NEPTUNE</t>
+  </si>
+  <si>
+    <t>ACHC</t>
+  </si>
+  <si>
+    <t>AGASSIZ COMMUNITY HEALTH CENTRE (CGH) 604.703.2030</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>COTTAGE PAVILION (ARHCC) 604.870.7999</t>
+  </si>
+  <si>
+    <t>MISSION HOME HEALTH OFFICE (MMH) 604.814.5520</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>MARGARET FULTON (LGH) 604-904-3550</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1217,23 +1255,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1269,23 +1290,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1461,10 +1465,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1501,7 +1505,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1515,7 +1519,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1529,7 +1533,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,7 +1547,7 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,7 +1561,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,7 +1575,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1599,7 +1603,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1613,7 +1617,7 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1627,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1641,7 +1645,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1655,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1669,7 +1673,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1683,7 +1687,7 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1697,7 +1701,7 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1711,7 +1715,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1725,7 +1729,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1739,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,7 +1757,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,7 +1771,7 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,7 +1785,7 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,7 +1799,7 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1809,7 +1813,7 @@
         <v>202</v>
       </c>
       <c r="D24" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1823,7 +1827,7 @@
         <v>202</v>
       </c>
       <c r="D25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1837,7 +1841,7 @@
         <v>202</v>
       </c>
       <c r="D26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1851,7 +1855,7 @@
         <v>202</v>
       </c>
       <c r="D27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1865,7 +1869,7 @@
         <v>202</v>
       </c>
       <c r="D28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1879,7 +1883,7 @@
         <v>202</v>
       </c>
       <c r="D29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,7 +1897,7 @@
         <v>243</v>
       </c>
       <c r="D30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,7 +1911,7 @@
         <v>243</v>
       </c>
       <c r="D31" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1921,78 +1925,78 @@
         <v>243</v>
       </c>
       <c r="D32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>312</v>
+      </c>
+      <c r="B33" t="s">
         <v>313</v>
       </c>
-      <c r="B33" t="s">
-        <v>314</v>
-      </c>
       <c r="C33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D34" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D36" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D36"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="87" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="87" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,16 +2044,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>353</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2321,69 +2325,66 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>355</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" t="s">
-        <v>201</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>348</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>351</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -2391,50 +2392,50 @@
       <c r="D25" t="s">
         <v>6</v>
       </c>
+      <c r="F25" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>199</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
         <v>199</v>
@@ -2442,139 +2443,139 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>349</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>350</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C32" t="s">
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
-        <v>201</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -2585,30 +2586,30 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F40" t="s">
         <v>201</v>
@@ -2616,10 +2617,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
@@ -2630,10 +2631,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
         <v>16</v>
@@ -2644,201 +2645,201 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
         <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
-      </c>
-      <c r="F44" t="s">
-        <v>201</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
         <v>16</v>
       </c>
-      <c r="D45" t="s">
-        <v>3</v>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
         <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>347</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>356</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
         <v>16</v>
       </c>
-      <c r="E48" t="s">
-        <v>189</v>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F49" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C51" t="s">
         <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
         <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C53" t="s">
         <v>16</v>
       </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" t="s">
-        <v>201</v>
+      <c r="E53" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C54" t="s">
         <v>16</v>
       </c>
-      <c r="E54" t="s">
-        <v>191</v>
+      <c r="D54" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C56" t="s">
         <v>16</v>
@@ -2849,10 +2850,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B57" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
@@ -2860,163 +2861,154 @@
       <c r="D57" t="s">
         <v>1</v>
       </c>
-      <c r="F57" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C58" t="s">
         <v>16</v>
       </c>
-      <c r="E58" t="s">
-        <v>187</v>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B59" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
       </c>
-      <c r="D59" t="s">
-        <v>1</v>
-      </c>
       <c r="E59" t="s">
-        <v>192</v>
-      </c>
-      <c r="F59" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C60" t="s">
         <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>3</v>
-      </c>
-      <c r="F60" t="s">
-        <v>199</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B61" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
       </c>
       <c r="D61" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
         <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B63" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C63" t="s">
         <v>16</v>
       </c>
-      <c r="D63" t="s">
-        <v>5</v>
+      <c r="E63" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B64" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C64" t="s">
         <v>16</v>
       </c>
       <c r="D64" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B65" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C65" t="s">
         <v>16</v>
       </c>
       <c r="D65" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" t="s">
-        <v>194</v>
+        <v>3</v>
+      </c>
+      <c r="F65" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B66" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
-      </c>
-      <c r="F66" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B67" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C67" t="s">
         <v>16</v>
@@ -3027,10 +3019,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B68" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C68" t="s">
         <v>16</v>
@@ -3041,196 +3033,194 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C69" t="s">
         <v>16</v>
       </c>
+      <c r="D69" t="s">
+        <v>5</v>
+      </c>
       <c r="E69" t="s">
-        <v>185</v>
+        <v>194</v>
+      </c>
+      <c r="F69" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B70" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C70" t="s">
         <v>16</v>
       </c>
       <c r="D70" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E70" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C71" t="s">
         <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="F71" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B72" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C72" t="s">
         <v>16</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>165</v>
+      </c>
+      <c r="B74" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>167</v>
+      </c>
+      <c r="B75" t="s">
+        <v>168</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>169</v>
+      </c>
+      <c r="B76" t="s">
+        <v>170</v>
+      </c>
+      <c r="C76" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>173</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B78" t="s">
         <v>174</v>
       </c>
-      <c r="C73" t="s">
-        <v>16</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="E76" s="4"/>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="5" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>202</v>
+        <v>16</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>211</v>
+        <v>7</v>
       </c>
       <c r="E79" s="4"/>
-      <c r="F79" s="5"/>
+      <c r="F79" s="4"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>202</v>
+        <v>16</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>204</v>
+        <v>5</v>
       </c>
       <c r="E80" s="4"/>
-      <c r="F80" s="5"/>
+      <c r="F80" s="4"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>202</v>
@@ -3243,10 +3233,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>202</v>
@@ -3261,10 +3251,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>202</v>
@@ -3279,42 +3269,42 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>202</v>
@@ -3323,80 +3313,82 @@
         <v>211</v>
       </c>
       <c r="E86" s="4"/>
-      <c r="F86" s="5" t="s">
-        <v>270</v>
-      </c>
+      <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E87" s="4"/>
-      <c r="F87" s="5"/>
+      <c r="F87" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E88" s="4"/>
-      <c r="F88" s="5"/>
+      <c r="F88" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>202</v>
@@ -3411,44 +3403,42 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E92" s="4"/>
-      <c r="F92" s="5" t="s">
-        <v>270</v>
-      </c>
+      <c r="F92" s="5"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="C93" s="4" t="s">
+      <c r="A93" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C93" s="5" t="s">
         <v>202</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>202</v>
@@ -3457,32 +3447,30 @@
         <v>204</v>
       </c>
       <c r="E94" s="4"/>
-      <c r="F94" s="5" t="s">
-        <v>270</v>
-      </c>
+      <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>202</v>
@@ -3491,16 +3479,14 @@
         <v>211</v>
       </c>
       <c r="E96" s="4"/>
-      <c r="F96" s="5" t="s">
-        <v>270</v>
-      </c>
+      <c r="F96" s="5"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>202</v>
@@ -3515,10 +3501,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>202</v>
@@ -3533,62 +3519,60 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E99" s="4"/>
-      <c r="F99" s="5" t="s">
-        <v>270</v>
-      </c>
+      <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E100" s="4"/>
-      <c r="F100" s="5"/>
+      <c r="F100" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E101" s="4"/>
-      <c r="F101" s="5" t="s">
-        <v>270</v>
-      </c>
+      <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>202</v>
@@ -3603,10 +3587,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>202</v>
@@ -3615,110 +3599,120 @@
         <v>211</v>
       </c>
       <c r="E103" s="4"/>
-      <c r="F103" s="5"/>
+      <c r="F103" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>271</v>
+        <v>212</v>
       </c>
       <c r="E104" s="4"/>
-      <c r="F104" s="5"/>
+      <c r="F104" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="F105" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E105" s="4"/>
+      <c r="F105" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>271</v>
+        <v>203</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="5"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>271</v>
+        <v>203</v>
       </c>
       <c r="E107" s="4"/>
-      <c r="F107" s="5"/>
+      <c r="F107" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>271</v>
+        <v>211</v>
       </c>
       <c r="E108" s="4"/>
-      <c r="F108" s="5"/>
+      <c r="F108" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>271</v>
+        <v>211</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="5"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>243</v>
@@ -3731,92 +3725,90 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D111" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="E111" s="4"/>
-      <c r="F111" s="5" t="s">
-        <v>275</v>
-      </c>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F111" s="5"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4" t="s">
-        <v>273</v>
-      </c>
+      <c r="D112" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E112" s="4"/>
       <c r="F112" s="5"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4" t="s">
-        <v>273</v>
-      </c>
+      <c r="D113" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E113" s="4"/>
       <c r="F113" s="5"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4" t="s">
-        <v>273</v>
-      </c>
+      <c r="D114" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E114" s="4"/>
       <c r="F114" s="5"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D115" s="4"/>
-      <c r="E115" s="4" t="s">
-        <v>273</v>
-      </c>
+      <c r="D115" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E115" s="4"/>
       <c r="F115" s="5"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>243</v>
@@ -3829,10 +3821,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>243</v>
@@ -3840,19 +3832,17 @@
       <c r="D117" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="E117" s="4" t="s">
-        <v>273</v>
-      </c>
+      <c r="E117" s="4"/>
       <c r="F117" s="5" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>243</v>
@@ -3865,10 +3855,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>243</v>
@@ -3881,267 +3871,382 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="4"/>
+      <c r="E120" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F120" s="5"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D122" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="E120" s="4"/>
-      <c r="F120" s="5"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="C122" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D122" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5" t="s">
-        <v>339</v>
-      </c>
+      <c r="E122" s="4"/>
+      <c r="F122" s="5"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
+      <c r="A123" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C124" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D124" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5" t="s">
-        <v>339</v>
-      </c>
+      <c r="A124" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F124" s="5"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D125" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5" t="s">
-        <v>340</v>
-      </c>
+      <c r="A125" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F125" s="5"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D126" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E126" s="5"/>
+      <c r="A126" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E126" s="4"/>
       <c r="F126" s="5"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E128" s="5"/>
-      <c r="F128" s="5"/>
+      <c r="F128" s="5" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E130" s="5"/>
-      <c r="F130" s="5"/>
+      <c r="F130" s="5" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="F137" s="5"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B138" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="B131" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D131" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="E131" s="5"/>
-      <c r="F131" s="5"/>
+      <c r="C138" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F131" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:F138"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D75</xm:sqref>
+          <xm:sqref>D2:D80</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$29</xm:f>
           </x14:formula1>
-          <xm:sqref>F76:F103</xm:sqref>
+          <xm:sqref>F81:F109</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$24:$B$28</xm:f>
           </x14:formula1>
-          <xm:sqref>D76:D103</xm:sqref>
+          <xm:sqref>D81:D109</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$32</xm:f>
           </x14:formula1>
-          <xm:sqref>F104:F120</xm:sqref>
+          <xm:sqref>F110:F126</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$31</xm:f>
           </x14:formula1>
-          <xm:sqref>E104:E120</xm:sqref>
+          <xm:sqref>E110:E126</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$30</xm:f>
           </x14:formula1>
-          <xm:sqref>D104:D120</xm:sqref>
+          <xm:sqref>D110:D126</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Cost Centres'!$B$15:$B$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E80</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Cost Centres'!$B$22:$B$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F80</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$35:$B$36</xm:f>
           </x14:formula1>
-          <xm:sqref>F121:F131</xm:sqref>
+          <xm:sqref>F127:F138</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost Centres'!$B$33:$B$34</xm:f>
           </x14:formula1>
-          <xm:sqref>D121:D131</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
-          <x14:formula1>
-            <xm:f>'Cost Centres'!$B$15:$B$21</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E75</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
-            <xm:f>'Cost Centres'!$B$22:$B$23</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F75</xm:sqref>
+          <xm:sqref>D127:D138</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>